<commit_message>
some anas and preparation
</commit_message>
<xml_diff>
--- a/docs/labeling/规则.xlsx
+++ b/docs/labeling/规则.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongjustin/Documents/Text2Scene/Text2Scene/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongjustin/Documents/Text2Scene/Text2Scene/docs/labeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009AEA35-AF2C-C647-8B98-4953E0E34560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8CBB6C-4F0A-A047-97A6-3F7266D66B13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="460" windowWidth="22200" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="185">
   <si>
     <t>抱枕 书 剪影</t>
   </si>
@@ -866,6 +866,9 @@
   </si>
   <si>
     <t>work</t>
+  </si>
+  <si>
+    <t>avatar</t>
   </si>
 </sst>
 </file>
@@ -1277,6 +1280,57 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1293,57 +1347,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1623,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="123" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="F35" zoomScale="125" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1647,61 +1650,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="58" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="59"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="30" customHeight="1">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="58" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="59"/>
-      <c r="G3" s="58" t="s">
+      <c r="F3" s="64"/>
+      <c r="G3" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="58" t="s">
+      <c r="H3" s="67"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="59"/>
+      <c r="K3" s="64"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
@@ -1775,43 +1778,43 @@
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:16" ht="30" customHeight="1">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="52" t="s">
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="70"/>
     </row>
     <row r="9" spans="1:16" ht="30" customHeight="1">
       <c r="A9" s="4" t="s">
@@ -1832,11 +1835,11 @@
       <c r="F9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
       <c r="J9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1884,73 +1887,73 @@
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
     </row>
     <row r="14" spans="1:16" ht="32">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="56" t="s">
+      <c r="H14" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="64" t="s">
+      <c r="I14" s="73"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="L14" s="57"/>
-      <c r="M14" s="64" t="s">
+      <c r="L14" s="53"/>
+      <c r="M14" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="N14" s="57"/>
-      <c r="O14" s="73" t="s">
+      <c r="N14" s="53"/>
+      <c r="O14" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="P14" s="73"/>
+      <c r="P14" s="62"/>
     </row>
     <row r="15" spans="1:16" ht="16">
-      <c r="H15" s="70" t="s">
+      <c r="H15" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="70" t="s">
+      <c r="I15" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="71"/>
-      <c r="K15" s="72" t="s">
+      <c r="J15" s="60"/>
+      <c r="K15" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="L15" s="71" t="s">
+      <c r="L15" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="72" t="s">
+      <c r="M15" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="N15" s="71" t="s">
+      <c r="N15" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="O15" s="63" t="s">
+      <c r="O15" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="P15" s="63" t="s">
+      <c r="P15" s="51" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="16">
-      <c r="H16" s="70"/>
+      <c r="H16" s="59"/>
       <c r="I16" s="26" t="s">
         <v>108</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="K16" s="72"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="71"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
     </row>
     <row r="17" spans="1:16" ht="16">
       <c r="C17" t="s">
@@ -2283,20 +2286,20 @@
       <c r="E37" t="s">
         <v>60</v>
       </c>
-      <c r="H37" s="65" t="s">
+      <c r="H37" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="67"/>
-      <c r="L37" s="68" t="s">
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="M37" s="67"/>
-      <c r="N37" s="69" t="s">
+      <c r="M37" s="56"/>
+      <c r="N37" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="O37" s="69"/>
+      <c r="O37" s="58"/>
     </row>
     <row r="38" spans="1:15" ht="16">
       <c r="C38" t="s">
@@ -2352,12 +2355,12 @@
       </c>
     </row>
     <row r="40" spans="1:15" ht="16">
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
       <c r="H40" s="13" t="s">
         <v>111</v>
       </c>
@@ -2714,6 +2717,9 @@
       <c r="K58" s="38"/>
       <c r="L58" s="46"/>
       <c r="M58" s="38"/>
+      <c r="N58" s="43" t="s">
+        <v>184</v>
+      </c>
       <c r="O58" s="11" t="s">
         <v>148</v>
       </c>
@@ -2902,6 +2908,20 @@
   </sheetData>
   <autoFilter ref="N15:N16" xr:uid="{E51DBCA8-5D8A-284C-8E28-22CF8951A6BA}"/>
   <mergeCells count="28">
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="P15:P16"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="M14:N14"/>
@@ -2916,20 +2936,6 @@
     <mergeCell ref="N15:N16"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="O15:O16"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A7:M7"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>